<commit_message>
Accounted for updated mortgage cost
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasmansfield/repos/household-money/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F1FD5-909E-0E47-8E24-1C73AEE0C8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FAFDB5-E848-E642-8981-6676F4AB37D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="4280" windowWidth="28040" windowHeight="17440" xr2:uid="{180D1295-64EC-7148-8EDB-A24A3B608AD2}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,11 +507,11 @@
         <v>8</v>
       </c>
       <c r="O1">
-        <v>1500</v>
+        <v>1633</v>
       </c>
       <c r="P1">
         <f>SUM(O1:O12)</f>
-        <v>2135</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -560,14 +560,14 @@
       </c>
       <c r="H3">
         <f>-P1</f>
-        <v>-2135</v>
+        <v>-2268</v>
       </c>
       <c r="I3">
         <v>-3000</v>
       </c>
       <c r="J3">
         <f>SUM(G3:I3)</f>
-        <v>2065</v>
+        <v>1932</v>
       </c>
       <c r="N3" t="s">
         <v>10</v>
@@ -640,11 +640,11 @@
       </c>
       <c r="J6">
         <f>J3*(1/3)</f>
-        <v>688.33333333333326</v>
+        <v>644</v>
       </c>
       <c r="K6">
         <f>J3*(2/3)</f>
-        <v>1376.6666666666665</v>
+        <v>1288</v>
       </c>
       <c r="L6" t="s">
         <v>16</v>
@@ -663,11 +663,11 @@
       </c>
       <c r="J7">
         <f>J6/4</f>
-        <v>172.08333333333331</v>
+        <v>161</v>
       </c>
       <c r="K7">
         <f>K6/4</f>
-        <v>344.16666666666663</v>
+        <v>322</v>
       </c>
       <c r="L7" t="s">
         <v>17</v>
@@ -718,11 +718,11 @@
       </c>
       <c r="J10">
         <f>J7+J9</f>
-        <v>422.08333333333331</v>
+        <v>411</v>
       </c>
       <c r="K10">
         <f>K7+K9</f>
-        <v>844.16666666666663</v>
+        <v>822</v>
       </c>
       <c r="L10" t="s">
         <v>20</v>

</xml_diff>